<commit_message>
1) 3 fogli comunicanti 2) subset definition 3) PCA è rotta
</commit_message>
<xml_diff>
--- a/data/shape_index_analysis.xlsx
+++ b/data/shape_index_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Gabri\Dev\repositories\git-hub\statistics-project-spotify\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matteo2/Documents/statistics-project-spotify/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468D512A-7736-4483-B1A7-836B48B54179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153A88FE-5817-0947-A8C4-9D482FC05374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{B09597DF-D22F-4E19-9985-B9224707B013}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B09597DF-D22F-4E19-9985-B9224707B013}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +110,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,19 +141,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -155,7 +187,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -455,17 +487,33 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.73046875" customWidth="1"/>
-    <col min="2" max="2" width="13.265625" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
@@ -502,435 +550,436 @@
         <v>15</v>
       </c>
       <c r="S1" s="2"/>
-      <c r="T1" t="s">
+      <c r="T1" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="U1" s="3"/>
       <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>-2.3309419999999998</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>7.3535700000000004</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>-0.196996</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>2.243506</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>1.0687739999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>4.3383370000000001</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>1.849793</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <v>6.6526630000000004</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="5">
         <v>-0.67822950000000004</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="5">
         <v>3.7753809999999999</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <v>2.3113890000000001</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="5">
         <v>6.7757519999999998</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <v>0.6468119</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="5">
         <v>3.2435529999999999</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="5">
         <v>-0.2379735</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="5">
         <v>1.9812099999999999</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="5">
         <v>0.48758459999999998</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="5">
         <v>1.432261</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="5">
         <v>2.3581530000000002</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="5">
         <v>10.446059999999999</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="5">
         <v>4.3489430000000002</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="5">
         <v>27.59712</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>-0.57801069999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>1.9635750000000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>-0.1713295</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>2.6311450000000001</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>0.3583112</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>2.2495750000000001</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>2.1316989999999998</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="5">
         <v>7.5157109999999996</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="5">
         <v>-0.9871394</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="5">
         <v>4.8644109999999996</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="5">
         <v>5.6648519999999998</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="5">
         <v>38.386690000000002</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <v>0.50371489999999997</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="5">
         <v>2.9942609999999998</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="5">
         <v>-0.1599768</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="5">
         <v>1.921565</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="5">
         <v>1.6242570000000001</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="5">
         <v>3.929627</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="5">
         <v>1.781782</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="5">
         <v>7.2062900000000001</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="5">
         <v>0.40327079999999998</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="5">
         <v>2.88896</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>0.87734279999999998</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>2.4359649999999999</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>-0.27359450000000002</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>2.5196719999999999</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>-0.36963119999999999</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>2.2594189999999998</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>2.2107380000000001</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>8.2284579999999998</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="5">
         <v>-1.5019499999999999</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>7.460464</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <v>4.5010839999999996</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <v>32.237900000000003</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="5">
         <v>0.54104790000000003</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="5">
         <v>2.8554460000000002</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="5">
         <v>-0.21108399999999999</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="5">
         <v>1.958996</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="5">
         <v>2.3304649999999998</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="5">
         <v>6.956925</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="5">
         <v>1.1157710000000001</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="5">
         <v>6.2826019999999998</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="5">
         <v>0.62170859999999994</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="5">
         <v>3.2051940000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>1.0508960000000001</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>2.8247719999999998</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>-0.27243279999999997</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>2.6982360000000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>-0.69200989999999996</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <v>2.8138480000000001</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>2.2199089999999999</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <v>8.6961689999999994</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="5">
         <v>-2.4754480000000001</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>12.88378</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>3.0329380000000001</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="5">
         <v>16.752960000000002</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="5">
         <v>0.41886479999999998</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="5">
         <v>2.5015869999999998</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="5">
         <v>-8.0646969999999998E-2</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="5">
         <v>1.9885010000000001</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="5">
         <v>2.9966140000000001</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="5">
         <v>10.592000000000001</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="5">
         <v>1.4383280000000001</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="5">
         <v>8.5517400000000006</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="5">
         <v>0.73669039999999997</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="5">
         <v>3.2794620000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>1.1330249999999999</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>3.0846260000000001</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>-0.56648810000000005</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>3.3930150000000001</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>-0.68904589999999999</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>3.1610520000000002</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>2.2544200000000001</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="5">
         <v>8.8660370000000004</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="5">
         <v>-3.2165469999999998</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>17.67361</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="5">
         <v>2.3418320000000001</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="5">
         <v>10.15325</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <v>0.1061566</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="5">
         <v>3.0564589999999998</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="5">
         <v>0.1590965</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="5">
         <v>2.1705990000000002</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="5">
         <v>3.3208350000000002</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="5">
         <v>12.613110000000001</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="5">
         <v>1.6013850000000001</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="5">
         <v>10.537430000000001</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="5">
         <v>-0.96873699999999996</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="5">
         <v>8.7302820000000008</v>
       </c>
     </row>
@@ -947,7 +996,612 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="L1:M1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B3:B7">
+    <cfRule type="dataBar" priority="25">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4CFE9850-15D3-F345-9F8D-56D6EC633716}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C7">
+    <cfRule type="dataBar" priority="19">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FEB23007-D76B-9C45-9895-A50DFDB32FB2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D7">
+    <cfRule type="dataBar" priority="23">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3C5E103C-1FC5-BF4A-9985-19E7261A3465}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="dataBar" priority="22">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9F6B81F8-2EC7-2944-90D1-E73D543E498E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F7">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7E232A66-E2BA-7349-B601-4C1C06182C1C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E7">
+    <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2046A05F-11C4-FA47-8411-21EBC6F1D5CC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G7">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{996B2E93-7B0D-1D4D-95B8-A0F0AA1724AD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I7">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A23F32C3-E1C7-564A-A780-C2193C0636DA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K7">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6932F4C4-E1F5-C64F-A01A-07E210A53249}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M7">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F8F3EEDF-F37C-0449-85FF-9890CFCA5BB2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O7">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FBF0A97C-3031-824C-9143-1B66A2B42140}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q7">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D69FA989-D1C2-844E-90D8-16B772D34B72}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S7">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1AF765C2-E5FA-7D4D-9A59-BE589A92FE39}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:U7">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FC4502CB-7A75-5840-A8C1-4B3204A68D88}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3:W7">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7ED52B32-CAE9-9C4A-86B9-6BFCB836E24A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H7">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C2794D59-22C2-3146-8145-7A6009AE1188}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J7">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8F641B76-3DC0-C74B-8378-6718AC1B0525}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L7">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{60E7688C-943F-F544-8488-2BC3F611A98B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N7">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E264297E-CCC1-124C-9F06-2AC63F6562CB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P7">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{31620A7B-ADBB-0B4A-976A-DBBECD22295E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3:R7">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0DAC9FD5-425F-C54F-BB0A-AF3459CF7D82}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T7">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F6527272-491E-1249-8ECD-8A39A507C56D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V7">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1F038E6D-0592-684E-BF66-370C075FFA20}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4CFE9850-15D3-F345-9F8D-56D6EC633716}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B3:B7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FEB23007-D76B-9C45-9895-A50DFDB32FB2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C3:C7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3C5E103C-1FC5-BF4A-9985-19E7261A3465}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D3:D7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9F6B81F8-2EC7-2944-90D1-E73D543E498E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7E232A66-E2BA-7349-B601-4C1C06182C1C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F3:F7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2046A05F-11C4-FA47-8411-21EBC6F1D5CC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E3:E7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{996B2E93-7B0D-1D4D-95B8-A0F0AA1724AD}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G3:G7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A23F32C3-E1C7-564A-A780-C2193C0636DA}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I3:I7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6932F4C4-E1F5-C64F-A01A-07E210A53249}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3:K7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F8F3EEDF-F37C-0449-85FF-9890CFCA5BB2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FBF0A97C-3031-824C-9143-1B66A2B42140}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O3:O7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D69FA989-D1C2-844E-90D8-16B772D34B72}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>Q3:Q7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1AF765C2-E5FA-7D4D-9A59-BE589A92FE39}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S3:S7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FC4502CB-7A75-5840-A8C1-4B3204A68D88}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U3:U7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7ED52B32-CAE9-9C4A-86B9-6BFCB836E24A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W3:W7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C2794D59-22C2-3146-8145-7A6009AE1188}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H3:H7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8F641B76-3DC0-C74B-8378-6718AC1B0525}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J3:J7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{60E7688C-943F-F544-8488-2BC3F611A98B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L3:L7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E264297E-CCC1-124C-9F06-2AC63F6562CB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N3:N7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{31620A7B-ADBB-0B4A-976A-DBBECD22295E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0DAC9FD5-425F-C54F-BB0A-AF3459CF7D82}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R3:R7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F6527272-491E-1249-8ECD-8A39A507C56D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>T3:T7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1F038E6D-0592-684E-BF66-370C075FFA20}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V3:V7</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>